<commit_message>
More on ACDynamicStabilityManager 2
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/IRON_CANARD_LOOP2_DYN/WEIGHTS/Weights.xlsx
+++ b/JPADSandBox_v2/out/IRON_CANARD_LOOP2_DYN/WEIGHTS/Weights.xlsx
@@ -116,37 +116,37 @@
     <t>WEIGHT ESTIMATION METHODS COMPARISON</t>
   </si>
   <si>
+    <t>ROSKAM</t>
+  </si>
+  <si>
     <t>JENKINSON</t>
   </si>
   <si>
+    <t>RAYMER</t>
+  </si>
+  <si>
+    <t>TORENBEEK_2013</t>
+  </si>
+  <si>
+    <t>SADRAEY</t>
+  </si>
+  <si>
     <t>KROO</t>
   </si>
   <si>
     <t>NICOLAI_1984</t>
   </si>
   <si>
-    <t>RAYMER</t>
-  </si>
-  <si>
-    <t>ROSKAM</t>
-  </si>
-  <si>
     <t>TORENBEEK_1976</t>
   </si>
   <si>
-    <t>SADRAEY</t>
-  </si>
-  <si>
-    <t>TORENBEEK_2013</t>
-  </si>
-  <si>
     <t>TORENBEEK_1982</t>
   </si>
   <si>
+    <t>HOWE</t>
+  </si>
+  <si>
     <t>NICOLAI_2013</t>
-  </si>
-  <si>
-    <t>HOWE</t>
   </si>
   <si>
     <t>Total Reference Mass</t>
@@ -1009,10 +1009,10 @@
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>18196.0</v>
+        <v>11693.0</v>
       </c>
       <c r="D8" t="n">
-        <v>220.11123450399845</v>
+        <v>105.70788442818497</v>
       </c>
     </row>
     <row r="9">
@@ -1023,10 +1023,10 @@
         <v>6</v>
       </c>
       <c r="C9" t="n">
-        <v>6642.0</v>
+        <v>18196.0</v>
       </c>
       <c r="D9" t="n">
-        <v>16.84869309604076</v>
+        <v>220.11123450399845</v>
       </c>
     </row>
     <row r="10">
@@ -1037,10 +1037,10 @@
         <v>6</v>
       </c>
       <c r="C10" t="n">
-        <v>8593.0</v>
+        <v>5962.0</v>
       </c>
       <c r="D10" t="n">
-        <v>51.1714573583677</v>
+        <v>4.8858639323389035</v>
       </c>
     </row>
     <row r="11">
@@ -1051,10 +1051,10 @@
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>5962.0</v>
+        <v>7277.0</v>
       </c>
       <c r="D11" t="n">
-        <v>4.8858639323389035</v>
+        <v>28.019864447438813</v>
       </c>
     </row>
     <row r="12">
@@ -1065,10 +1065,10 @@
         <v>6</v>
       </c>
       <c r="C12" t="n">
-        <v>11693.0</v>
+        <v>5745.0</v>
       </c>
       <c r="D12" t="n">
-        <v>105.70788442818497</v>
+        <v>1.0683140374516944</v>
       </c>
     </row>
     <row r="13">
@@ -1079,10 +1079,10 @@
         <v>6</v>
       </c>
       <c r="C13" t="n">
-        <v>7797.0</v>
+        <v>6642.0</v>
       </c>
       <c r="D13" t="n">
-        <v>37.167910278504934</v>
+        <v>16.84869309604076</v>
       </c>
     </row>
     <row r="14">
@@ -1093,10 +1093,10 @@
         <v>6</v>
       </c>
       <c r="C14" t="n">
-        <v>5745.0</v>
+        <v>8593.0</v>
       </c>
       <c r="D14" t="n">
-        <v>1.0683140374516944</v>
+        <v>51.1714573583677</v>
       </c>
     </row>
     <row r="15">
@@ -1107,10 +1107,10 @@
         <v>6</v>
       </c>
       <c r="C15" t="n">
-        <v>7277.0</v>
+        <v>7797.0</v>
       </c>
       <c r="D15" t="n">
-        <v>28.019864447438813</v>
+        <v>37.167910278504934</v>
       </c>
     </row>
   </sheetData>
@@ -1203,16 +1203,16 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>5604.0</v>
+        <v>6319.0</v>
       </c>
       <c r="D8" t="n">
-        <v>-6.9926545041826005</v>
+        <v>4.873914380455059</v>
       </c>
     </row>
     <row r="9">
@@ -1223,10 +1223,10 @@
         <v>6</v>
       </c>
       <c r="C9" t="n">
-        <v>6319.0</v>
+        <v>4911.0</v>
       </c>
       <c r="D9" t="n">
-        <v>4.873914380455059</v>
+        <v>-18.494098192369872</v>
       </c>
     </row>
     <row r="10">
@@ -1245,16 +1245,16 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>4911.0</v>
+        <v>5604.0</v>
       </c>
       <c r="D11" t="n">
-        <v>-18.494098192369872</v>
+        <v>-6.9926545041826005</v>
       </c>
     </row>
   </sheetData>
@@ -1347,86 +1347,86 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>961.0</v>
+        <v>1718.0</v>
       </c>
       <c r="D8" t="n">
-        <v>47.0112381882031</v>
+        <v>162.8150959493579</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
       </c>
       <c r="C9" t="n">
-        <v>1006.0</v>
+        <v>1784.0</v>
       </c>
       <c r="D9" t="n">
-        <v>53.89521916475788</v>
+        <v>172.91160138163823</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
       </c>
       <c r="C10" t="n">
-        <v>514.0</v>
+        <v>961.0</v>
       </c>
       <c r="D10" t="n">
-        <v>-21.369639512241</v>
+        <v>47.0112381882031</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>1718.0</v>
+        <v>619.0</v>
       </c>
       <c r="D11" t="n">
-        <v>162.8150959493579</v>
+        <v>-5.307017233613191</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
       </c>
       <c r="C12" t="n">
-        <v>619.0</v>
+        <v>1746.0</v>
       </c>
       <c r="D12" t="n">
-        <v>-5.307017233613191</v>
+        <v>167.0984618903253</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
       </c>
       <c r="C13" t="n">
-        <v>1784.0</v>
+        <v>514.0</v>
       </c>
       <c r="D13" t="n">
-        <v>172.91160138163823</v>
+        <v>-21.369639512241</v>
       </c>
     </row>
     <row r="14">
@@ -1437,24 +1437,24 @@
         <v>6</v>
       </c>
       <c r="C14" t="n">
-        <v>882.0</v>
+        <v>1006.0</v>
       </c>
       <c r="D14" t="n">
-        <v>34.92602714047361</v>
+        <v>53.89521916475788</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B15" t="s">
         <v>6</v>
       </c>
       <c r="C15" t="n">
-        <v>1746.0</v>
+        <v>882.0</v>
       </c>
       <c r="D15" t="n">
-        <v>167.0984618903253</v>
+        <v>34.92602714047361</v>
       </c>
     </row>
   </sheetData>
@@ -1547,49 +1547,49 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>538.0</v>
+        <v>1017.0</v>
       </c>
       <c r="D8" t="n">
-        <v>-17.698182991411787</v>
+        <v>55.57797007013794</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
       </c>
       <c r="C9" t="n">
-        <v>483.0</v>
+        <v>1784.0</v>
       </c>
       <c r="D9" t="n">
-        <v>-26.11193751831207</v>
+        <v>172.91160138163823</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
       </c>
       <c r="C10" t="n">
-        <v>1017.0</v>
+        <v>538.0</v>
       </c>
       <c r="D10" t="n">
-        <v>55.57797007013794</v>
+        <v>-17.698182991411787</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
@@ -1609,10 +1609,10 @@
         <v>6</v>
       </c>
       <c r="C12" t="n">
-        <v>1784.0</v>
+        <v>773.0</v>
       </c>
       <c r="D12" t="n">
-        <v>172.91160138163823</v>
+        <v>18.251495441707597</v>
       </c>
     </row>
     <row r="13">
@@ -1623,24 +1623,24 @@
         <v>6</v>
       </c>
       <c r="C13" t="n">
-        <v>503.0</v>
+        <v>483.0</v>
       </c>
       <c r="D13" t="n">
-        <v>-23.05239041762106</v>
+        <v>-26.11193751831207</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B14" t="s">
         <v>6</v>
       </c>
       <c r="C14" t="n">
-        <v>773.0</v>
+        <v>503.0</v>
       </c>
       <c r="D14" t="n">
-        <v>18.251495441707597</v>
+        <v>-23.05239041762106</v>
       </c>
     </row>
   </sheetData>
@@ -1733,91 +1733,91 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>315.0</v>
+        <v>430.0</v>
       </c>
       <c r="D8" t="n">
-        <v>-44.58395313873405</v>
+        <v>-24.352697935414742</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
       </c>
       <c r="C9" t="n">
-        <v>328.0</v>
+        <v>464.0</v>
       </c>
       <c r="D9" t="n">
-        <v>-42.29694168096752</v>
+        <v>-18.371283353563815</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
       </c>
       <c r="C10" t="n">
-        <v>217.0</v>
+        <v>315.0</v>
       </c>
       <c r="D10" t="n">
-        <v>-61.8245010511279</v>
+        <v>-44.58395313873405</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>430.0</v>
+        <v>230.0</v>
       </c>
       <c r="D11" t="n">
-        <v>-24.352697935414742</v>
+        <v>-59.53748959336137</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
       </c>
       <c r="C12" t="n">
-        <v>230.0</v>
+        <v>217.0</v>
       </c>
       <c r="D12" t="n">
-        <v>-59.53748959336137</v>
+        <v>-61.8245010511279</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
       </c>
       <c r="C13" t="n">
-        <v>464.0</v>
+        <v>328.0</v>
       </c>
       <c r="D13" t="n">
-        <v>-18.371283353563815</v>
+        <v>-42.29694168096752</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B14" t="s">
         <v>6</v>
@@ -1943,7 +1943,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
@@ -2001,7 +2001,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
@@ -2161,7 +2161,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
@@ -2219,7 +2219,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
@@ -2342,7 +2342,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
@@ -2361,7 +2361,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
@@ -2377,7 +2377,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>

</xml_diff>